<commit_message>
CMIP5 mappings and typo in concentrations.py
</commit_message>
<xml_diff>
--- a/mappings/aerosol-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/aerosol-cmip5-to-cmip6-mappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t xml:space="preserve">CMIP5 component [&gt; process]</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Aerosol Scheme Scope</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.key_properties.scheme_scope</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aerosol Time Step Framework &gt; Method</t>
   </si>
   <si>
@@ -49,16 +52,31 @@
     <t xml:space="preserve">Aerosol Time Step Framework &gt; Time Step</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.key_properties.timestep_framework.integrated_timestep</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basic Approximations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmip6.aerosol.key_properties.basic_approximations</t>
   </si>
   <si>
     <t xml:space="preserve">Family Approach</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.key_properties.family_approach</t>
+  </si>
+  <si>
     <t xml:space="preserve">List Of Prognostic Variables</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.key_properties.prognostic_variables_form</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number Of Tracers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmip6.aerosol.key_properties.number_of_tracers</t>
   </si>
   <si>
     <t xml:space="preserve">Aerosols &gt; Emission &amp; Concentration</t>
@@ -112,7 +130,13 @@
     <t xml:space="preserve">Concentrations &gt; Prescribed Lower Boundary</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.concentrations.prescribed_lower_boundary</t>
+  </si>
+  <si>
     <t xml:space="preserve">Concentrations &gt; Prescribed Upper Boundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmip6.aerosol.concentrations.prescribed_upper_boundary</t>
   </si>
   <si>
     <t xml:space="preserve">Concentrations &gt; Prescribed Within Atmos</t>
@@ -130,6 +154,9 @@
     <t xml:space="preserve">Aerosol Scheme &gt; Bulk Species</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.model.bulk_scheme_species</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aerosol Scheme &gt; Framework</t>
   </si>
   <si>
@@ -145,19 +172,31 @@
     <t xml:space="preserve">Aerosol Scheme &gt; Scheme Type</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.model.scheme_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aerosol Scheme &gt; Species</t>
   </si>
   <si>
     <t xml:space="preserve">Coupling With</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.model.coupling</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gas Phase Precursors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmip6.aerosol.model.gas_phase_precursors</t>
   </si>
   <si>
     <t xml:space="preserve">Ocean Biogeochemical Coupling</t>
   </si>
   <si>
     <t xml:space="preserve">Processes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmip6.aerosol.model.processes</t>
   </si>
   <si>
     <t xml:space="preserve">Vegetation Model Coupling</t>
@@ -169,10 +208,19 @@
     <t xml:space="preserve">Convection</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.transport.convention</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mass Conservation</t>
   </si>
   <si>
+    <t xml:space="preserve">cmip6.aerosol.transport.mass_conservation_scheme</t>
+  </si>
+  <si>
     <t xml:space="preserve">Method Detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmip6.aerosol.transport.overview</t>
   </si>
   <si>
     <t xml:space="preserve">Scheme Type</t>
@@ -354,16 +402,17 @@
   </sheetPr>
   <dimension ref="A1:IU50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="60.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.4642857142857"/>
-    <col collapsed="false" hidden="false" max="255" min="4" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.6683673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="63.7244897959184"/>
+    <col collapsed="false" hidden="false" max="255" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="256" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="23" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -636,7 +685,9 @@
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
       <c r="F2" s="0"/>
@@ -895,10 +946,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
@@ -1158,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="0"/>
@@ -1419,9 +1470,11 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="D5" s="0"/>
       <c r="E5" s="0"/>
       <c r="F5" s="0"/>
@@ -1680,9 +1733,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
@@ -1941,9 +1996,11 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
@@ -2202,9 +2259,11 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
@@ -2463,9 +2522,11 @@
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
@@ -2978,10 +3039,10 @@
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="0"/>
@@ -3239,10 +3300,10 @@
     </row>
     <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="0"/>
@@ -3500,10 +3561,10 @@
     </row>
     <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="0"/>
@@ -3761,10 +3822,10 @@
     </row>
     <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="0"/>
@@ -4022,10 +4083,10 @@
     </row>
     <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="0"/>
@@ -4283,10 +4344,10 @@
     </row>
     <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="0"/>
@@ -4544,10 +4605,10 @@
     </row>
     <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="0"/>
@@ -4805,10 +4866,10 @@
     </row>
     <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="0"/>
@@ -5066,10 +5127,10 @@
     </row>
     <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="0"/>
@@ -5327,10 +5388,10 @@
     </row>
     <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="0"/>
@@ -5588,10 +5649,10 @@
     </row>
     <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="0"/>
@@ -5849,10 +5910,10 @@
     </row>
     <row r="22" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="0"/>
@@ -6110,10 +6171,10 @@
     </row>
     <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="0"/>
@@ -6371,10 +6432,10 @@
     </row>
     <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="0"/>
@@ -6632,10 +6693,10 @@
     </row>
     <row r="25" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="0"/>
@@ -6893,12 +6954,14 @@
     </row>
     <row r="26" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D26" s="0"/>
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
@@ -7154,12 +7217,14 @@
     </row>
     <row r="27" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="D27" s="0"/>
       <c r="E27" s="0"/>
       <c r="F27" s="0"/>
@@ -7415,10 +7480,10 @@
     </row>
     <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="0"/>
@@ -7933,10 +7998,10 @@
     </row>
     <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="0"/>
@@ -8194,10 +8259,10 @@
     </row>
     <row r="31" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="0"/>
@@ -8455,12 +8520,14 @@
     </row>
     <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
-      <c r="C32" s="6"/>
+      <c r="C32" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="D32" s="0"/>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
@@ -8716,10 +8783,10 @@
     </row>
     <row r="33" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="0"/>
@@ -8977,10 +9044,10 @@
     </row>
     <row r="34" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="0"/>
@@ -9238,10 +9305,10 @@
     </row>
     <row r="35" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C35" s="6"/>
       <c r="D35" s="0"/>
@@ -9499,10 +9566,10 @@
     </row>
     <row r="36" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C36" s="6"/>
       <c r="D36" s="0"/>
@@ -9760,12 +9827,14 @@
     </row>
     <row r="37" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
-      <c r="C37" s="6"/>
+      <c r="C37" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="D37" s="0"/>
       <c r="E37" s="0"/>
       <c r="F37" s="0"/>
@@ -10021,10 +10090,10 @@
     </row>
     <row r="38" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38" s="0"/>
@@ -10282,12 +10351,14 @@
     </row>
     <row r="39" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="D39" s="0"/>
       <c r="E39" s="0"/>
       <c r="F39" s="0"/>
@@ -10543,12 +10614,14 @@
     </row>
     <row r="40" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="D40" s="0"/>
       <c r="E40" s="0"/>
       <c r="F40" s="0"/>
@@ -10804,10 +10877,10 @@
     </row>
     <row r="41" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="0"/>
@@ -11065,12 +11138,14 @@
     </row>
     <row r="42" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="D42" s="0"/>
       <c r="E42" s="0"/>
       <c r="F42" s="0"/>
@@ -11326,10 +11401,10 @@
     </row>
     <row r="43" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="0"/>
@@ -11844,55 +11919,61 @@
     </row>
     <row r="45" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
-      <c r="C45" s="6"/>
+      <c r="C45" s="7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
-      <c r="C46" s="6"/>
+      <c r="C46" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
-      <c r="C47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C48" s="6"/>
     </row>
     <row r="49" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C49" s="6"/>
     </row>
     <row r="50" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C50" s="6"/>
     </row>

</xml_diff>